<commit_message>
incorporated estimated fix times into data frame
</commit_message>
<xml_diff>
--- a/est_fix_time.xlsx
+++ b/est_fix_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAX\python\comp_issues\visualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC61F69C-C82A-4C28-9ED3-795AB3C53178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1731228D-51D0-441F-821E-CAE2C9A89F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Damaged</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Warped</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Not Available</t>
   </si>
 </sst>
 </file>
@@ -825,7 +825,7 @@
   <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,22 +842,22 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -874,10 +874,10 @@
         <v>1.5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G2" s="2">
         <f>ROUND(D2+IF(E2="y",1/3,0)+IF(F2="y",3.5,0),1)</f>
@@ -892,17 +892,17 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D3" s="2">
         <f>ROUND(AVERAGE(D2,D4:D10),1)</f>
         <v>0.9</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G66" si="0">ROUND(D3+IF(E3="y",1/3,0)+IF(F3="y",3.5,0),1)</f>
@@ -917,16 +917,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
@@ -941,16 +941,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
@@ -965,16 +965,16 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
         <v>0.5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -989,16 +989,16 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
         <v>0.25</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
@@ -1013,16 +1013,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
@@ -1037,16 +1037,16 @@
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -1061,16 +1061,16 @@
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
@@ -1082,19 +1082,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -1106,19 +1106,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
@@ -1130,19 +1130,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
@@ -1154,19 +1154,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
@@ -1178,10 +1178,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
@@ -1198,7 +1198,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
@@ -1218,10 +1218,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D17" s="2">
         <f>AVERAGE(D15:D16,D18:D20)</f>
@@ -1239,10 +1239,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -1259,10 +1259,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2">
         <v>4</v>
@@ -1279,10 +1279,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2">
         <v>4</v>
@@ -1299,10 +1299,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D21" s="2">
         <f>7/8</f>
@@ -1320,7 +1320,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>1</v>
@@ -1340,10 +1340,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2">
         <v>0.75</v>
@@ -1360,10 +1360,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2">
         <v>0.75</v>
@@ -1380,10 +1380,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D25" s="2">
         <f>ROUND(AVERAGE(D21:D24,D26:D27),1)</f>
@@ -1401,10 +1401,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="2">
         <v>0.75</v>
@@ -1421,10 +1421,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="2">
         <v>0.5</v>
@@ -1441,10 +1441,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D28" s="2">
         <v>1.5</v>
@@ -1461,10 +1461,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2">
         <v>1.5</v>
@@ -1481,10 +1481,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="2">
         <v>1.5</v>
@@ -1501,10 +1501,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D31" s="2">
         <v>1.5</v>
@@ -1521,10 +1521,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="2">
         <v>1.5</v>
@@ -1541,10 +1541,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -1561,10 +1561,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
@@ -1581,10 +1581,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -1601,10 +1601,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="2">
         <v>0</v>
@@ -1621,10 +1621,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -1641,10 +1641,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D38" s="2">
         <v>0.625</v>
@@ -1661,10 +1661,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="2">
         <v>0.5</v>
@@ -1681,10 +1681,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40" s="2">
         <v>8</v>
@@ -1701,10 +1701,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" s="2">
         <v>8</v>
@@ -1721,10 +1721,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
@@ -1741,10 +1741,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D43" s="2">
         <v>2</v>
@@ -1761,10 +1761,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D44" s="2">
         <v>2</v>
@@ -1781,10 +1781,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
@@ -1801,10 +1801,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
@@ -1821,10 +1821,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" s="2">
         <v>0</v>
@@ -1841,10 +1841,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
@@ -1861,10 +1861,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2">
         <v>0</v>
@@ -1881,10 +1881,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="2">
         <v>0</v>
@@ -1901,10 +1901,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D51" s="2">
         <v>0</v>
@@ -1921,10 +1921,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D52" s="2">
         <v>0</v>
@@ -1941,10 +1941,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D53" s="2">
         <v>0</v>
@@ -1961,10 +1961,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D54" s="2">
         <v>0</v>
@@ -1981,10 +1981,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55" s="2">
         <v>0</v>
@@ -2001,10 +2001,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" s="2">
         <v>0.5</v>
@@ -2021,10 +2021,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D57" s="2">
         <v>0.5</v>
@@ -2041,10 +2041,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D58" s="2">
         <v>0.5</v>
@@ -2061,10 +2061,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D59" s="2">
         <v>0.5</v>
@@ -2081,10 +2081,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D60" s="2">
         <v>0.5</v>
@@ -2101,10 +2101,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61" s="2">
         <v>0.58299999999999996</v>
@@ -2121,10 +2121,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
@@ -2141,10 +2141,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D63" s="2">
         <v>1</v>
@@ -2161,10 +2161,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2">
         <v>0.58299999999999996</v>
@@ -2181,10 +2181,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" s="2">
         <v>1</v>
@@ -2201,10 +2201,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D66" s="2">
         <f>ROUND(AVERAGE(D62:D65,D67:D69),1)</f>
@@ -2222,10 +2222,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D67" s="2">
         <v>0.58299999999999996</v>
@@ -2242,10 +2242,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -2262,10 +2262,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D69" s="2">
         <v>0.58299999999999996</v>
@@ -2282,10 +2282,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D70" s="2">
         <v>0.5</v>
@@ -2302,10 +2302,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D71" s="2">
         <v>0.5</v>
@@ -2322,10 +2322,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D72" s="2">
         <v>0.5</v>
@@ -2342,10 +2342,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D73" s="2">
         <v>0.5</v>
@@ -2362,10 +2362,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74" s="2">
         <v>0.5</v>
@@ -2382,10 +2382,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D75" s="2">
         <v>0.5</v>
@@ -2402,10 +2402,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D76" s="2">
         <v>0.625</v>
@@ -2422,10 +2422,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D77" s="2">
         <v>3.5</v>
@@ -2442,10 +2442,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
@@ -2462,10 +2462,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D79" s="2">
         <f>ROUND(AVERAGE(D76:D78,D80:D83),1)</f>
@@ -2483,10 +2483,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D80" s="2">
         <v>0.625</v>
@@ -2503,10 +2503,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D81" s="2">
         <v>0.625</v>
@@ -2523,10 +2523,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D82" s="2">
         <v>0.625</v>
@@ -2543,10 +2543,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
@@ -2563,10 +2563,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D84" s="2">
         <v>0.25</v>
@@ -2583,10 +2583,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D85" s="2">
         <v>8</v>
@@ -2603,10 +2603,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D86" s="2">
         <f>AVERAGE(D84:D85)</f>
@@ -2624,10 +2624,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D87" s="2">
         <v>0</v>
@@ -2644,10 +2644,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D88" s="2">
         <v>0</v>
@@ -2664,10 +2664,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D89" s="2">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>1</v>
@@ -2704,10 +2704,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D91" s="2">
         <f>ROUND(AVERAGE(D90,D92:D96),1)</f>
@@ -2725,10 +2725,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D92" s="2">
         <v>0</v>
@@ -2745,10 +2745,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D93" s="2">
         <v>0</v>
@@ -2765,10 +2765,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D94" s="2">
         <v>0</v>
@@ -2785,10 +2785,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D95" s="2">
         <v>0.33</v>
@@ -2805,10 +2805,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D96" s="2">
         <v>0</v>
@@ -2825,10 +2825,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D97" s="2">
         <v>2</v>
@@ -2845,10 +2845,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D98" s="2">
         <v>0.75</v>
@@ -2865,10 +2865,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D99" s="2">
         <f>ROUND(AVERAGE(D97:D98,D100:D103),1)</f>
@@ -2886,10 +2886,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D100" s="2">
         <v>0.5</v>
@@ -2906,10 +2906,10 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D101" s="2">
         <v>1</v>
@@ -2926,10 +2926,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D102" s="2">
         <v>0.5</v>
@@ -2946,10 +2946,10 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D103" s="2">
         <v>1</v>
@@ -2966,10 +2966,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D104" s="2">
         <v>1.125</v>
@@ -2986,10 +2986,10 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D105" s="2">
         <f>ROUND(1/12,1)</f>
@@ -3007,10 +3007,10 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D106" s="2">
         <v>1.125</v>
@@ -3027,10 +3027,10 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D107" s="2">
         <f>ROUND(AVERAGE(D104:D106,D108:D109),1)</f>
@@ -3048,10 +3048,10 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D108" s="2">
         <v>1.125</v>
@@ -3068,10 +3068,10 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D109" s="2">
         <v>1.5</v>
@@ -3088,10 +3088,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="D110" s="2">
         <v>0.5</v>
@@ -3108,10 +3108,10 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D111" s="2">
         <v>0.5</v>
@@ -3128,10 +3128,10 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D112" s="2">
         <v>0.5</v>
@@ -3148,10 +3148,10 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D113" s="2">
         <v>0.5</v>
@@ -3168,10 +3168,10 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D114" s="2">
         <v>0.5</v>
@@ -3188,7 +3188,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>1</v>
@@ -3208,10 +3208,10 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D116" s="2">
         <v>0.33</v>
@@ -3228,10 +3228,10 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D117" s="2">
         <v>0.33</v>
@@ -3248,10 +3248,10 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D118" s="2">
         <v>0.33</v>
@@ -3268,10 +3268,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D119" s="2">
         <v>0.33</v>
@@ -3288,10 +3288,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D120" s="2">
         <v>0.33</v>
@@ -3308,10 +3308,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D121" s="2">
         <v>0.33</v>
@@ -3328,10 +3328,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D122" s="2">
         <v>0.33</v>
@@ -3348,10 +3348,10 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D123" s="2">
         <v>0.33</v>
@@ -3368,10 +3368,10 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D124" s="2">
         <v>0.33</v>
@@ -3388,10 +3388,10 @@
         <v>123</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D125" s="2">
         <v>1</v>
@@ -3408,10 +3408,10 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D126" s="2">
         <v>1</v>
@@ -3428,10 +3428,10 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D127" s="2">
         <v>1.25</v>
@@ -3448,10 +3448,10 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D128" s="2">
         <f>ROUND(AVERAGE(D125:D127,D129:D131),1)</f>
@@ -3469,10 +3469,10 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D129" s="2">
         <v>1</v>
@@ -3489,10 +3489,10 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D130" s="2">
         <v>0</v>
@@ -3509,10 +3509,10 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D131" s="2">
         <v>1.25</v>
@@ -3529,10 +3529,10 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D132" s="2">
         <v>0</v>
@@ -3549,10 +3549,10 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D133" s="2">
         <f>ROUND(AVERAGE(D132,D134:D140),1)</f>
@@ -3570,10 +3570,10 @@
         <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D134" s="2">
         <v>0.5</v>
@@ -3590,10 +3590,10 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D135" s="2">
         <v>3.75</v>
@@ -3610,10 +3610,10 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D136" s="2">
         <v>0</v>
@@ -3630,10 +3630,10 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D137" s="2">
         <v>3.75</v>
@@ -3650,10 +3650,10 @@
         <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D138" s="2">
         <v>3.75</v>
@@ -3670,10 +3670,10 @@
         <v>137</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D139" s="2">
         <v>1.5</v>
@@ -3690,10 +3690,10 @@
         <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D140" s="2">
         <v>1.5</v>
@@ -3710,10 +3710,10 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D141" s="2">
         <v>8</v>
@@ -3730,10 +3730,10 @@
         <v>140</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D142" s="2">
         <v>8</v>
@@ -3750,10 +3750,10 @@
         <v>141</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D143" s="2">
         <v>0</v>
@@ -3770,10 +3770,10 @@
         <v>142</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D144" s="2">
         <v>0.58299999999999996</v>
@@ -3790,10 +3790,10 @@
         <v>143</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D145" s="2">
         <v>0</v>
@@ -3810,10 +3810,10 @@
         <v>144</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D146" s="2">
         <v>0.16600000000000001</v>
@@ -3830,10 +3830,10 @@
         <v>145</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D147" s="2">
         <v>0.5</v>
@@ -3850,10 +3850,10 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D148" s="2">
         <f>ROUND(AVERAGE(D143:D147,D149:D150),1)</f>
@@ -3871,10 +3871,10 @@
         <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D149" s="2">
         <v>0</v>
@@ -3891,10 +3891,10 @@
         <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D150" s="2">
         <v>0.5</v>
@@ -3911,10 +3911,10 @@
         <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D151" s="2">
         <v>1.75</v>
@@ -3931,10 +3931,10 @@
         <v>150</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D152" s="2">
         <v>1</v>
@@ -3951,10 +3951,10 @@
         <v>151</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D153" s="2">
         <v>1.75</v>
@@ -3971,10 +3971,10 @@
         <v>152</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D154" s="2">
         <f>ROUND(AVERAGE(D151:D153,D155:D157),1)</f>
@@ -3992,10 +3992,10 @@
         <v>153</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D155" s="2">
         <v>1.04</v>
@@ -4012,10 +4012,10 @@
         <v>154</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D156" s="2">
         <v>0.28999999999999998</v>
@@ -4032,10 +4032,10 @@
         <v>155</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D157" s="2">
         <v>0.125</v>
@@ -4052,10 +4052,10 @@
         <v>156</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D158" s="2">
         <v>0</v>
@@ -4072,10 +4072,10 @@
         <v>157</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D159" s="2">
         <v>0.375</v>
@@ -4092,10 +4092,10 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D160" s="2">
         <v>0.75</v>
@@ -4112,10 +4112,10 @@
         <v>159</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D161" s="2">
         <v>0</v>
@@ -4132,10 +4132,10 @@
         <v>160</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C162" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D162" s="2">
         <v>0</v>
@@ -4152,10 +4152,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D163" s="2">
         <v>0</v>
@@ -4172,10 +4172,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D164" s="2">
         <v>0.125</v>
@@ -4192,10 +4192,10 @@
         <v>163</v>
       </c>
       <c r="B165" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D165" s="2">
         <v>0.54</v>
@@ -4212,7 +4212,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>1</v>
@@ -4232,10 +4232,10 @@
         <v>165</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D167" s="2">
         <f>ROUND(AVERAGE(D164:D166),1)</f>
@@ -4253,10 +4253,10 @@
         <v>166</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D168" s="2">
         <v>0</v>
@@ -4273,10 +4273,10 @@
         <v>167</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D169" s="2">
         <v>0</v>
@@ -4293,10 +4293,10 @@
         <v>168</v>
       </c>
       <c r="B170" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="D170" s="2">
         <v>0.75</v>
@@ -4313,10 +4313,10 @@
         <v>169</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D171" s="2">
         <v>0.75</v>
@@ -4333,10 +4333,10 @@
         <v>170</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D172" s="2">
         <v>0.75</v>
@@ -4353,10 +4353,10 @@
         <v>171</v>
       </c>
       <c r="B173" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D173" s="2">
         <v>0</v>
@@ -4373,10 +4373,10 @@
         <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D174" s="2">
         <v>0</v>
@@ -4393,10 +4393,10 @@
         <v>173</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D175" s="2">
         <v>0</v>
@@ -4413,10 +4413,10 @@
         <v>174</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D176" s="2">
         <v>0</v>
@@ -4433,10 +4433,10 @@
         <v>175</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D177" s="2">
         <v>0</v>

</xml_diff>